<commit_message>
Added script for ExtentReport and Log4j
</commit_message>
<xml_diff>
--- a/KotakHL_Lead/TestData/TestData_LeadDetails.xlsx
+++ b/KotakHL_Lead/TestData/TestData_LeadDetails.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16665" windowHeight="7470" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Output" sheetId="2" r:id="rId2"/>
+    <sheet name="TestScenario" sheetId="3" r:id="rId1"/>
+    <sheet name="HLNewLead" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Output" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:J22"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
   <si>
     <t>Username</t>
   </si>
@@ -135,9 +136,6 @@
     <t>PAN</t>
   </si>
   <si>
-    <t>CLNPK5929G</t>
-  </si>
-  <si>
     <t>DIGI HL</t>
   </si>
   <si>
@@ -168,9 +166,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Direct</t>
   </si>
   <si>
@@ -186,15 +181,9 @@
     <t>Auto</t>
   </si>
   <si>
-    <t>TestLead1</t>
-  </si>
-  <si>
     <t>Individual/Non-Individual</t>
   </si>
   <si>
-    <t>autoTestLead1@gmail.com</t>
-  </si>
-  <si>
     <t>Mobile No.</t>
   </si>
   <si>
@@ -240,28 +229,98 @@
     <t>Post Graduate</t>
   </si>
   <si>
-    <t>C:\\Users\\Vrunda Vibhute\\eclipse-workspace\\KotakHL_Lead\\TestData\\8.jpg</t>
-  </si>
-  <si>
     <t>Document Upload</t>
   </si>
   <si>
-    <t>8087531111</t>
-  </si>
-  <si>
-    <t>00101993</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>Create HL New Lead</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>Relationship Manager</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>1200000</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>9898989898</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>00102419</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Sent to LOS</t>
+    <t>Documents Pending</t>
+  </si>
+  <si>
+    <t>22/04/2022 11:17 AM</t>
+  </si>
+  <si>
+    <t>C:\Users\Vrunda Vibhute\git\KMBSeleniumJavaFramework1\KotakHL_Lead\TestData\\8.jpg</t>
+  </si>
+  <si>
+    <t>00102446</t>
+  </si>
+  <si>
+    <t>New Lead</t>
+  </si>
+  <si>
+    <t>22/04/2022 5:32 PM</t>
+  </si>
+  <si>
+    <t>Follow-Up New</t>
+  </si>
+  <si>
+    <t>22/04/2022 5:33 PM</t>
+  </si>
+  <si>
+    <t>Appointment Fixed</t>
+  </si>
+  <si>
+    <t>22/04/2022 5:34 PM</t>
+  </si>
+  <si>
+    <t>22/04/2022 5:35 PM</t>
+  </si>
+  <si>
+    <t>25/04/2022 12:06 PM</t>
+  </si>
+  <si>
+    <t>25/04/2022 12:07 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,15 +351,21 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -308,22 +373,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,294 +720,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.85546875" customWidth="1"/>
-    <col min="24" max="25" width="16.7109375" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" customWidth="1"/>
-    <col min="28" max="28" width="18" customWidth="1"/>
-    <col min="29" max="29" width="17.7109375" customWidth="1"/>
-    <col min="30" max="30" width="19.42578125" customWidth="1"/>
-    <col min="31" max="31" width="34.42578125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="21.7109375" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" customWidth="1"/>
-    <col min="34" max="34" width="26.7109375" customWidth="1"/>
-    <col min="35" max="35" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15" customWidth="1"/>
-    <col min="38" max="38" width="12.85546875" customWidth="1"/>
-    <col min="39" max="39" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="75.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="49.140625"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125"/>
+    <col min="4" max="4" customWidth="true" width="16.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AP3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AM6" sqref="AM6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="15" width="9.140625"/>
+    <col min="2" max="2" customWidth="true" style="15" width="22.42578125"/>
+    <col min="3" max="3" customWidth="true" style="15" width="12.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="15" width="9.42578125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="11.5703125"/>
+    <col min="6" max="6" customWidth="true" style="15" width="14.7109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="15" width="12.140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="14.28515625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="15" width="12.5703125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="15" width="10.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="15" width="10.5703125"/>
+    <col min="12" max="12" customWidth="true" style="15" width="12.28515625"/>
+    <col min="13" max="13" customWidth="true" style="15" width="25.0"/>
+    <col min="14" max="14" customWidth="true" style="15" width="16.28515625"/>
+    <col min="15" max="15" customWidth="true" style="15" width="30.7109375"/>
+    <col min="16" max="16" customWidth="true" style="15" width="12.85546875"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="15" width="14.5703125"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="15" width="18.28515625"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="15" width="12.85546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="15" width="12.0"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="15" width="14.5703125"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="15" width="14.7109375"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="15" width="35.85546875"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="15" width="61.7109375"/>
+    <col min="25" max="25" customWidth="true" style="15" width="17.85546875"/>
+    <col min="26" max="27" customWidth="true" style="15" width="16.7109375"/>
+    <col min="28" max="28" customWidth="true" style="15" width="15.5703125"/>
+    <col min="29" max="29" customWidth="true" style="15" width="11.140625"/>
+    <col min="30" max="30" customWidth="true" style="15" width="18.0"/>
+    <col min="31" max="31" customWidth="true" style="15" width="17.7109375"/>
+    <col min="32" max="32" customWidth="true" style="15" width="19.42578125"/>
+    <col min="33" max="33" customWidth="true" style="16" width="34.42578125"/>
+    <col min="34" max="34" customWidth="true" style="15" width="21.7109375"/>
+    <col min="35" max="35" customWidth="true" style="15" width="13.140625"/>
+    <col min="36" max="36" customWidth="true" style="15" width="26.7109375"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="15" width="13.5703125"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="15" width="13.42578125"/>
+    <col min="39" max="39" customWidth="true" style="15" width="15.0"/>
+    <col min="40" max="40" customWidth="true" style="15" width="12.85546875"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" style="15" width="13.5703125"/>
+    <col min="42" max="42" customWidth="true" style="15" width="91.42578125"/>
+    <col min="43" max="16384" style="15" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="11" t="str">
+        <f ca="1">Sheet1!A2</f>
+        <v>HLNew Lead 545</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="9" t="str">
+        <f ca="1">Sheet1!C2</f>
+        <v>HLNewLead545@gmail.com</v>
+      </c>
+      <c r="P2" s="9" t="str">
+        <f ca="1">Sheet1!D2</f>
+        <v>15111978</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="9" t="str">
+        <f ca="1">Sheet1!E2</f>
+        <v>ILKKH9438F</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF2" s="9">
+        <v>400068</v>
+      </c>
+      <c r="AG2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AH2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI2" s="9" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
+        <v>Male</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AM2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AN1" s="4" t="s">
-        <v>75</v>
+      <c r="AP2" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="2">
-        <v>8087531111</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="2">
-        <v>14071991</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1500000</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1200000</v>
-      </c>
-      <c r="R2" s="2">
-        <v>36</v>
-      </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>400068</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>74</v>
-      </c>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="N3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -923,55 +1084,143 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.28515625"/>
+    <col min="2" max="2" customWidth="true" width="21.85546875"/>
+    <col min="3" max="3" customWidth="true" width="31.0"/>
+    <col min="4" max="4" customWidth="true" width="25.0"/>
+    <col min="5" max="5" customWidth="true" width="17.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="str">
+        <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
+        <v>HLNew Lead 545</v>
+      </c>
+      <c r="B2" s="2">
+        <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
+        <v>9346792812</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
+        <v>HLNewLead545@gmail.com</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
+        <v>15111978</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
+        <v>ILKKH9438F</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="11.42578125"/>
+    <col min="2" max="2" customWidth="true" width="24.140625"/>
+    <col min="3" max="3" customWidth="true" width="17.0"/>
+    <col min="4" max="4" customWidth="true" width="25.85546875"/>
+    <col min="5" max="5" customWidth="true" width="21.7109375"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="6">
-        <v>44662.631944444445</v>
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>